<commit_message>
updated data + viz
</commit_message>
<xml_diff>
--- a/data/simplified_book_list.xlsx
+++ b/data/simplified_book_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aayushiverma/Documents/Github/My-Book-Stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02884F2-A45D-0542-9BB3-18BD75A7EBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC1DB84-E4F3-1F47-B5AB-F6C77EB8F8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="500" windowWidth="39620" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="goodreads_library_export" sheetId="1" r:id="rId1"/>
@@ -3322,8 +3322,8 @@
   <dimension ref="A1:P267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B240" sqref="B240"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I126" sqref="I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3338,7 +3338,7 @@
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" customWidth="1"/>
     <col min="12" max="13" width="10.6640625" customWidth="1"/>
     <col min="14" max="14" width="11.5" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" customWidth="1"/>
@@ -3424,9 +3424,8 @@
       <c r="J2">
         <v>1974</v>
       </c>
-      <c r="K2" t="e">
-        <f>YEAR(#REF!)</f>
-        <v>#REF!</v>
+      <c r="K2">
+        <v>2007</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -7785,7 +7784,7 @@
         <v>13</v>
       </c>
       <c r="I125">
-        <v>1656</v>
+        <v>2014</v>
       </c>
       <c r="J125">
         <v>2014</v>

</xml_diff>

<commit_message>
added office book list
</commit_message>
<xml_diff>
--- a/data/simplified_book_list.xlsx
+++ b/data/simplified_book_list.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aayushiverma/Documents/Github/My-Book-Stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A03B79-FACF-7F40-B6C1-1AC9080E2F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE4C6C5-427D-F646-B0A4-1FC5C9512D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="35100" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44680" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="goodreads_library_export" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">goodreads_library_export!$A$1:$M$1</definedName>
@@ -38,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="618">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="616">
   <si>
     <t>Author l-f</t>
   </si>
@@ -49,12 +45,6 @@
     <t>Additional Authors</t>
   </si>
   <si>
-    <t>ISBN</t>
-  </si>
-  <si>
-    <t>ISBN13</t>
-  </si>
-  <si>
     <t>Number of Pages</t>
   </si>
   <si>
@@ -1687,9 +1677,6 @@
     <t>INDIA, CAMBRIDGE</t>
   </si>
   <si>
-    <t>The universe next door</t>
-  </si>
-  <si>
     <t>In case of emergency</t>
   </si>
   <si>
@@ -1702,15 +1689,6 @@
     <t>Kowal, Mary Robinette</t>
   </si>
   <si>
-    <t>user_tags</t>
-  </si>
-  <si>
-    <t>ownership_status</t>
-  </si>
-  <si>
-    <t>user_genre</t>
-  </si>
-  <si>
     <t>physics</t>
   </si>
   <si>
@@ -1756,9 +1734,6 @@
     <t>history;biography;astronomy</t>
   </si>
   <si>
-    <t>fiction_status</t>
-  </si>
-  <si>
     <t>thriller</t>
   </si>
   <si>
@@ -1777,9 +1752,6 @@
     <t>Year Read</t>
   </si>
   <si>
-    <t>buy?</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -1789,9 +1761,6 @@
     <t>Bray, Libby</t>
   </si>
   <si>
-    <t>radio rebel</t>
-  </si>
-  <si>
     <t>Driftwood</t>
   </si>
   <si>
@@ -1807,9 +1776,6 @@
     <t>Mark Jones</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>Model Misfit</t>
   </si>
   <si>
@@ -1892,6 +1858,33 @@
   </si>
   <si>
     <t>Bhagat, Madhukur Kumar</t>
+  </si>
+  <si>
+    <t>Book Title</t>
+  </si>
+  <si>
+    <t>Radio Rebel</t>
+  </si>
+  <si>
+    <t>ISBN-10</t>
+  </si>
+  <si>
+    <t>ISBN-13</t>
+  </si>
+  <si>
+    <t>User Genre</t>
+  </si>
+  <si>
+    <t>Fiction Status</t>
+  </si>
+  <si>
+    <t>User Tags</t>
+  </si>
+  <si>
+    <t>Ownership Status</t>
+  </si>
+  <si>
+    <t>Buy?</t>
   </si>
 </sst>
 </file>
@@ -2763,11 +2756,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N271"/>
+  <dimension ref="A1:N286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K281" sqref="K281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2788,57 +2781,57 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>609</v>
+      </c>
+      <c r="E1" t="s">
+        <v>610</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="J1" t="s">
-        <v>556</v>
+        <v>611</v>
       </c>
       <c r="K1" t="s">
-        <v>572</v>
+        <v>612</v>
       </c>
       <c r="L1" t="s">
-        <v>554</v>
+        <v>613</v>
       </c>
       <c r="M1" t="s">
-        <v>555</v>
+        <v>614</v>
       </c>
       <c r="N1" t="s">
-        <v>579</v>
+        <v>615</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D2" t="str">
         <f>"0136042597"</f>
@@ -2861,27 +2854,27 @@
         <v>2023</v>
       </c>
       <c r="J2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L2" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D3" t="str">
         <f>"0128042915"</f>
@@ -2904,27 +2897,27 @@
         <v>2022</v>
       </c>
       <c r="J3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L3" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="str">
         <f>"1107492610"</f>
@@ -2947,24 +2940,24 @@
         <v>2018</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L4" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5" t="str">
         <f>"0767930487"</f>
@@ -2987,27 +2980,27 @@
         <v>2018</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L5" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6" t="str">
         <f>""</f>
@@ -3030,24 +3023,24 @@
         <v>2018</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L6" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B7" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D7" t="str">
         <f>"1107512824"</f>
@@ -3067,27 +3060,27 @@
         <v>2023</v>
       </c>
       <c r="J7" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L7" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B8" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C8" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D8" t="str">
         <f>"110845514X"</f>
@@ -3110,27 +3103,27 @@
         <v>2022</v>
       </c>
       <c r="J8" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L8" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="B9" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
       <c r="C9" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="D9" s="4">
         <v>1107492637</v>
@@ -3148,24 +3141,24 @@
         <v>2018</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L9" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B10" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D10" s="4">
         <v>312367465</v>
@@ -3191,10 +3184,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B11" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D11" t="str">
         <f>"0525476881"</f>
@@ -3221,10 +3214,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D12" t="str">
         <f>"0316166464"</f>
@@ -3252,10 +3245,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B13" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D13" t="str">
         <f>"0141384786"</f>
@@ -3282,10 +3275,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B14" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D14" t="str">
         <f>""</f>
@@ -3309,10 +3302,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B15" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D15" t="str">
         <f>""</f>
@@ -3339,10 +3332,10 @@
     </row>
     <row r="16" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B16" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D16" s="3">
         <v>1466440961</v>
@@ -3368,10 +3361,10 @@
     </row>
     <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B17" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D17" s="3">
         <v>1463768591</v>
@@ -3398,10 +3391,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B18" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D18" t="str">
         <f>"0957291205"</f>
@@ -3429,10 +3422,10 @@
     </row>
     <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B19" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D19" s="3">
         <v>1849163944</v>
@@ -3458,10 +3451,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B20" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D20" t="str">
         <f>"0545397367"</f>
@@ -3488,10 +3481,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B21" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D21" t="str">
         <f>""</f>
@@ -3518,10 +3511,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B22" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D22" t="str">
         <f>""</f>
@@ -3548,10 +3541,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B23" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D23" t="str">
         <f>""</f>
@@ -3578,10 +3571,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B24" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D24" t="str">
         <f>"1476792488"</f>
@@ -3608,10 +3601,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D25" t="str">
         <f>"1408725797"</f>
@@ -3633,15 +3626,15 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D26" t="str">
         <f>"0063216051"</f>
@@ -3663,15 +3656,15 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B27" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D27" t="str">
         <f>"1449371434"</f>
@@ -3694,27 +3687,27 @@
         <v>2023</v>
       </c>
       <c r="J27" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="L27" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B28" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C28" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D28" t="str">
         <f>""</f>
@@ -3741,10 +3734,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D29" t="str">
         <f>""</f>
@@ -3767,19 +3760,19 @@
         <v>2021</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="K29" s="1"/>
       <c r="N29" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B30" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D30" t="str">
         <f>"0517189607"</f>
@@ -3804,15 +3797,15 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="N30" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D31" t="str">
         <f>"0156632772"</f>
@@ -3835,19 +3828,19 @@
         <v>2021</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="K31" s="1"/>
       <c r="N31" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D32" t="str">
         <f>""</f>
@@ -3872,18 +3865,18 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="N32" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B33" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C33" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D33" t="str">
         <f>"1435122941"</f>
@@ -3910,10 +3903,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B34" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D34" t="str">
         <f>"0330397761"</f>
@@ -3937,13 +3930,13 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D35" t="str">
         <f>"0671687042"</f>
@@ -3966,18 +3959,18 @@
         <v>2020</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B36" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D36" t="str">
         <f>"0385732554"</f>
@@ -4004,13 +3997,13 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D37" t="str">
         <f>"1844806979"</f>
@@ -4034,15 +4027,15 @@
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D38" t="str">
         <f>"0790004054"</f>
@@ -4065,18 +4058,18 @@
         <v>2021</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B39" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D39" t="str">
         <f>""</f>
@@ -4098,18 +4091,18 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="N39" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B40" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C40" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D40" t="str">
         <f>""</f>
@@ -4132,16 +4125,16 @@
         <v>2023</v>
       </c>
       <c r="J40" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D41" t="str">
         <f>"039333810X"</f>
@@ -4164,21 +4157,21 @@
         <v>2015</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M41" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B42" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D42" t="str">
         <f>"0385735421"</f>
@@ -4205,10 +4198,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B43" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D43" t="str">
         <f>"0192718711"</f>
@@ -4235,10 +4228,10 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B44" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D44" t="str">
         <f>"3423708549"</f>
@@ -4262,10 +4255,10 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B45" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D45" t="str">
         <f>"033039908X"</f>
@@ -4292,10 +4285,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B46" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D46" t="str">
         <f>"0446610577"</f>
@@ -4322,10 +4315,10 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B47" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D47" t="str">
         <f>"043994998X"</f>
@@ -4345,16 +4338,16 @@
         <v>2015</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B48" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D48" t="str">
         <f>"0064473481"</f>
@@ -4381,10 +4374,10 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B49" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D49" t="str">
         <f>"1416907173"</f>
@@ -4411,13 +4404,13 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D50" t="str">
         <f>""</f>
@@ -4440,18 +4433,18 @@
         <v>2021</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B51" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D51" t="str">
         <f>""</f>
@@ -4476,15 +4469,15 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="N51" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D52" t="str">
         <f>"0316058254"</f>
@@ -4509,15 +4502,15 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="N52" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B53" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D53" t="str">
         <f>"0141317841"</f>
@@ -4544,10 +4537,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B54" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D54" t="str">
         <f>"038573283X"</f>
@@ -4574,10 +4567,10 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D55" t="str">
         <f>"2916238018"</f>
@@ -4600,16 +4593,16 @@
         <v>2021</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B56" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D56" t="str">
         <f>"0753461315"</f>
@@ -4636,10 +4629,10 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B57" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D57" t="str">
         <f>"0439951143"</f>
@@ -4666,10 +4659,10 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B58" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D58" t="str">
         <f>""</f>
@@ -4696,10 +4689,10 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B59" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D59" t="str">
         <f>""</f>
@@ -4726,10 +4719,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D60" t="str">
         <f>"1416949763"</f>
@@ -4756,10 +4749,10 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D61" t="str">
         <f>""</f>
@@ -4786,10 +4779,10 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B62" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D62" t="str">
         <f>"1416933484"</f>
@@ -4814,15 +4807,15 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="N62" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D63" t="str">
         <f>"0439871808"</f>
@@ -4849,10 +4842,10 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B64" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D64" t="str">
         <f>"1853409073"</f>
@@ -4879,10 +4872,10 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B65" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D65" t="str">
         <f>""</f>
@@ -4909,10 +4902,10 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D66" t="str">
         <f>"1250236401"</f>
@@ -4939,10 +4932,10 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B67" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D67" t="str">
         <f>"1599903016"</f>
@@ -4969,10 +4962,10 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B68" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D68" t="str">
         <f>"1416935584"</f>
@@ -4999,10 +4992,10 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D69" t="str">
         <f>"0764330667"</f>
@@ -5025,18 +5018,18 @@
         <v>2023</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B70" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D70" t="str">
         <f>"1921502363"</f>
@@ -5063,10 +5056,10 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B71" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D71" t="str">
         <f>"031253275X"</f>
@@ -5093,10 +5086,10 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B72" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D72" t="str">
         <f>""</f>
@@ -5123,10 +5116,10 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D73" t="str">
         <f>"1862918473"</f>
@@ -5153,10 +5146,10 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D74" t="str">
         <f>"141698643X"</f>
@@ -5183,10 +5176,10 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B75" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D75" t="str">
         <f>"0141325194"</f>
@@ -5213,10 +5206,10 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B76" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D76" t="str">
         <f>""</f>
@@ -5240,10 +5233,10 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B77" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D77" t="str">
         <f>""</f>
@@ -5270,10 +5263,10 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D78" t="str">
         <f>"1407105132"</f>
@@ -5300,10 +5293,10 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B79" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D79" t="str">
         <f>"1869508165"</f>
@@ -5330,10 +5323,10 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B80" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D80" t="str">
         <f>"1444900846"</f>
@@ -5360,13 +5353,13 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B81" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C81" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D81" t="str">
         <f>"1470008955"</f>
@@ -5393,10 +5386,10 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B82" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D82" t="str">
         <f>"141697170X"</f>
@@ -5423,10 +5416,10 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B83" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D83" t="str">
         <f>"0007326270"</f>
@@ -5451,15 +5444,15 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="N83" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B84" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D84" t="str">
         <f>"0373210086"</f>
@@ -5486,10 +5479,10 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B85" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D85" t="str">
         <f>"0312575939"</f>
@@ -5516,10 +5509,10 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B86" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D86" t="str">
         <f>"1536897345"</f>
@@ -5546,10 +5539,10 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B87" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D87" t="str">
         <f>"0732288401"</f>
@@ -5576,10 +5569,10 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B88" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D88" t="str">
         <f>""</f>
@@ -5606,10 +5599,10 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B89" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D89" t="str">
         <f>""</f>
@@ -5636,10 +5629,10 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B90" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D90" t="str">
         <f>""</f>
@@ -5666,10 +5659,10 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B91" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D91" t="str">
         <f>"057805339X"</f>
@@ -5696,10 +5689,10 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B92" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D92" t="str">
         <f>""</f>
@@ -5726,10 +5719,10 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B93" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D93" t="str">
         <f>""</f>
@@ -5756,10 +5749,10 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B94" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D94" t="str">
         <f>"1453778039"</f>
@@ -5786,10 +5779,10 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D95" t="str">
         <f>"1848879466"</f>
@@ -5812,18 +5805,18 @@
         <v>2020</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B96" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D96" t="str">
         <f>"1405282886"</f>
@@ -5850,10 +5843,10 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B97" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D97" t="str">
         <f>"1921759321"</f>
@@ -5880,10 +5873,10 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D98" t="str">
         <f>""</f>
@@ -5910,10 +5903,10 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B99" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D99" t="str">
         <f>"0007334060"</f>
@@ -5940,10 +5933,10 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B100" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D100" t="str">
         <f>"1595143971"</f>
@@ -5970,10 +5963,10 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B101" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D101" t="str">
         <f>""</f>
@@ -5997,10 +5990,10 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B102" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D102" t="str">
         <f>""</f>
@@ -6027,10 +6020,10 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B103" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D103" t="str">
         <f>""</f>
@@ -6057,10 +6050,10 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B104" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D104" t="str">
         <f>"1466459670"</f>
@@ -6087,10 +6080,10 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B105" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D105" t="str">
         <f>""</f>
@@ -6115,15 +6108,15 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
       <c r="N105" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B106" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D106" t="str">
         <f>""</f>
@@ -6144,10 +6137,10 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B107" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D107" t="str">
         <f>"1444757814"</f>
@@ -6174,10 +6167,10 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B108" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D108" t="str">
         <f>""</f>
@@ -6204,10 +6197,10 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B109" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D109" t="str">
         <f>""</f>
@@ -6231,10 +6224,10 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B110" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D110" t="str">
         <f>""</f>
@@ -6261,10 +6254,10 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B111" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D111" t="str">
         <f>""</f>
@@ -6291,10 +6284,10 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B112" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D112" t="str">
         <f>""</f>
@@ -6321,10 +6314,10 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B113" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D113" t="str">
         <f>""</f>
@@ -6351,10 +6344,10 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B114" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D114" t="str">
         <f>"1937085767"</f>
@@ -6381,10 +6374,10 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B115" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D115" t="str">
         <f>""</f>
@@ -6411,10 +6404,10 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B116" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D116" t="str">
         <f>"0984662103"</f>
@@ -6441,10 +6434,10 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B117" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D117" t="str">
         <f>""</f>
@@ -6471,10 +6464,10 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B118" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D118" t="str">
         <f>"0062085484"</f>
@@ -6501,10 +6494,10 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B119" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D119" t="str">
         <f>""</f>
@@ -6531,10 +6524,10 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B120" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D120" t="str">
         <f>""</f>
@@ -6558,10 +6551,10 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B121" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D121" t="str">
         <f>""</f>
@@ -6585,10 +6578,10 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B122" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D122" t="str">
         <f>""</f>
@@ -6615,10 +6608,10 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B123" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D123" t="str">
         <f>""</f>
@@ -6645,10 +6638,10 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B124" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D124" t="str">
         <f>""</f>
@@ -6672,10 +6665,10 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B125" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D125" t="str">
         <f>"0986915505"</f>
@@ -6702,10 +6695,10 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B126" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D126" t="str">
         <f>""</f>
@@ -6732,10 +6725,10 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B127" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D127" t="str">
         <f>"1466392509"</f>
@@ -6762,10 +6755,10 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B128" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D128" t="str">
         <f>"0983398038"</f>
@@ -6792,10 +6785,10 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B129" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D129" t="str">
         <f>""</f>
@@ -6822,10 +6815,10 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B130" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D130" t="str">
         <f>"1742692664"</f>
@@ -6852,10 +6845,10 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B131" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D131" t="str">
         <f>"0615535186"</f>
@@ -6882,10 +6875,10 @@
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B132" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D132" t="str">
         <f>""</f>
@@ -6912,13 +6905,13 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B133" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C133" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D133" t="str">
         <f>"1426207700"</f>
@@ -6941,18 +6934,18 @@
         <v>2021</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B134" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D134" t="str">
         <f>"098730786X"</f>
@@ -6979,10 +6972,10 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B135" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D135" t="str">
         <f>""</f>
@@ -7009,10 +7002,10 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B136" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D136" t="str">
         <f>""</f>
@@ -7039,10 +7032,10 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B137" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D137" t="str">
         <f>""</f>
@@ -7066,10 +7059,10 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B138" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D138" t="str">
         <f>""</f>
@@ -7096,10 +7089,10 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B139" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D139" t="str">
         <f>""</f>
@@ -7126,10 +7119,10 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B140" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D140" t="str">
         <f>""</f>
@@ -7156,10 +7149,10 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B141" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D141" t="str">
         <f>""</f>
@@ -7186,10 +7179,10 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B142" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D142" t="str">
         <f>""</f>
@@ -7216,10 +7209,10 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B143" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D143" t="str">
         <f>""</f>
@@ -7246,10 +7239,10 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B144" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D144" t="str">
         <f>"152380419X"</f>
@@ -7276,13 +7269,13 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B145" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C145" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D145" t="str">
         <f>""</f>
@@ -7309,10 +7302,10 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B146" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D146" t="str">
         <f>"1250012570"</f>
@@ -7339,10 +7332,10 @@
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B147" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D147" t="str">
         <f>""</f>
@@ -7369,10 +7362,10 @@
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B148" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D148" t="str">
         <f>"1475070373"</f>
@@ -7399,10 +7392,10 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B149" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D149" t="str">
         <f>""</f>
@@ -7426,10 +7419,10 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B150" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D150" t="str">
         <f>"077831345X"</f>
@@ -7456,10 +7449,10 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B151" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D151" t="str">
         <f>""</f>
@@ -7486,13 +7479,13 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B152" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C152" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D152" t="str">
         <f>"1452665524"</f>
@@ -7516,10 +7509,10 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B153" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D153" t="str">
         <f>"1250005647"</f>
@@ -7546,10 +7539,10 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B154" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D154" t="str">
         <f>""</f>
@@ -7576,10 +7569,10 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B155" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D155" t="str">
         <f>"0778313387"</f>
@@ -7606,10 +7599,10 @@
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B156" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D156" t="str">
         <f>"1599908727"</f>
@@ -7636,10 +7629,10 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B157" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D157" t="str">
         <f>"0375869549"</f>
@@ -7666,10 +7659,10 @@
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B158" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D158" t="str">
         <f>"0062059939"</f>
@@ -7694,15 +7687,15 @@
       <c r="J158" s="1"/>
       <c r="K158" s="1"/>
       <c r="N158" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B159" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D159" t="str">
         <f>""</f>
@@ -7729,10 +7722,10 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B160" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D160" t="str">
         <f>""</f>
@@ -7756,10 +7749,10 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B161" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D161" t="str">
         <f>""</f>
@@ -7786,10 +7779,10 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B162" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D162" t="str">
         <f>"1940534364"</f>
@@ -7816,10 +7809,10 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B163" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D163" t="str">
         <f>"0987484516"</f>
@@ -7846,10 +7839,10 @@
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B164" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D164" t="str">
         <f>""</f>
@@ -7873,10 +7866,10 @@
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B165" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D165" t="str">
         <f>"0988715309"</f>
@@ -7900,10 +7893,10 @@
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B166" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D166" t="str">
         <f>""</f>
@@ -7930,10 +7923,10 @@
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B167" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D167" t="str">
         <f>""</f>
@@ -7957,10 +7950,10 @@
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B168" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D168" t="str">
         <f>""</f>
@@ -7987,10 +7980,10 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B169" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D169" t="str">
         <f>"031620076X"</f>
@@ -8017,10 +8010,10 @@
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B170" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D170" t="str">
         <f>""</f>
@@ -8047,10 +8040,10 @@
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B171" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D171" t="str">
         <f>"1407124323"</f>
@@ -8077,10 +8070,10 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B172" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D172" t="str">
         <f>""</f>
@@ -8107,10 +8100,10 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B173" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D173" t="str">
         <f>""</f>
@@ -8134,10 +8127,10 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B174" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D174" t="str">
         <f>""</f>
@@ -8164,10 +8157,10 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B175" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D175" t="str">
         <f>"1471115992"</f>
@@ -8194,10 +8187,10 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B176" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D176" t="str">
         <f>""</f>
@@ -8224,10 +8217,10 @@
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B177" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D177" t="str">
         <f>"1489553207"</f>
@@ -8254,10 +8247,10 @@
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B178" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D178" t="str">
         <f>"1743315864"</f>
@@ -8284,10 +8277,10 @@
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B179" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D179" t="str">
         <f>""</f>
@@ -8314,10 +8307,10 @@
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B180" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D180" t="str">
         <f>"0812995325"</f>
@@ -8342,15 +8335,15 @@
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
       <c r="N180" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B181" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D181" t="str">
         <f>""</f>
@@ -8377,10 +8370,10 @@
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B182" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D182" t="str">
         <f>""</f>
@@ -8407,10 +8400,10 @@
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B183" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D183" t="str">
         <f>"0992452414"</f>
@@ -8437,10 +8430,10 @@
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B184" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D184" t="str">
         <f>"1338129384"</f>
@@ -8467,10 +8460,10 @@
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B185" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D185" t="str">
         <f>""</f>
@@ -8497,10 +8490,10 @@
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B186" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D186" t="str">
         <f>"1743317662"</f>
@@ -8527,10 +8520,10 @@
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B187" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D187" t="str">
         <f>""</f>
@@ -8554,10 +8547,10 @@
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B188" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D188" t="str">
         <f>"1500395447"</f>
@@ -8584,10 +8577,10 @@
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B189" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D189" t="str">
         <f>""</f>
@@ -8614,10 +8607,10 @@
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B190" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D190" t="str">
         <f>""</f>
@@ -8644,10 +8637,10 @@
     </row>
     <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B191" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D191" t="str">
         <f>"0373211090"</f>
@@ -8674,10 +8667,10 @@
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B192" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D192" t="str">
         <f>"0732297052"</f>
@@ -8704,10 +8697,10 @@
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B193" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D193" t="str">
         <f>""</f>
@@ -8734,10 +8727,10 @@
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B194" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D194" t="str">
         <f>"1444780107"</f>
@@ -8760,21 +8753,21 @@
         <v>2020</v>
       </c>
       <c r="J194" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K194" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="N194" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B195" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D195" t="str">
         <f>"1250043689"</f>
@@ -8797,18 +8790,18 @@
         <v>2021</v>
       </c>
       <c r="J195" s="1" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="K195" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B196" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D196" t="str">
         <f>"145491341X"</f>
@@ -8831,18 +8824,18 @@
         <v>2021</v>
       </c>
       <c r="J196" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K196" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B197" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D197" t="str">
         <f>"0804173524"</f>
@@ -8865,21 +8858,21 @@
         <v>2021</v>
       </c>
       <c r="J197" s="1" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="K197" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B198" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C198" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D198" t="str">
         <f>""</f>
@@ -8903,10 +8896,10 @@
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B199" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D199" t="str">
         <f>""</f>
@@ -8933,10 +8926,10 @@
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B200" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D200" t="str">
         <f>""</f>
@@ -8963,10 +8956,10 @@
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B201" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D201" t="str">
         <f>""</f>
@@ -8990,10 +8983,10 @@
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B202" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D202" t="str">
         <f>""</f>
@@ -9016,21 +9009,21 @@
         <v>2021</v>
       </c>
       <c r="J202" s="1" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="K202" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="N202" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B203" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D203" t="str">
         <f>""</f>
@@ -9053,21 +9046,21 @@
         <v>2021</v>
       </c>
       <c r="J203" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="K203" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="N203" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B204" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D204" t="str">
         <f>"1910258008"</f>
@@ -9090,24 +9083,24 @@
         <v>2021</v>
       </c>
       <c r="J204" s="1" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="K204" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="N204" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B205" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C205" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D205" t="str">
         <f>"1780288883"</f>
@@ -9131,18 +9124,18 @@
       </c>
       <c r="J205" s="1"/>
       <c r="K205" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="N205" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B206" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D206" t="str">
         <f>"0062314009"</f>
@@ -9168,13 +9161,13 @@
     </row>
     <row r="207" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B207" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C207" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D207" t="str">
         <f>"1335004882"</f>
@@ -9201,13 +9194,13 @@
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B208" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C208" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D208" t="str">
         <f>""</f>
@@ -9234,10 +9227,10 @@
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B209" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D209" t="str">
         <f>"0714871044"</f>
@@ -9261,15 +9254,15 @@
       </c>
       <c r="J209" s="1"/>
       <c r="K209" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B210" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D210" t="str">
         <f>"1101904224"</f>
@@ -9292,16 +9285,16 @@
         <v>2023</v>
       </c>
       <c r="J210" s="1" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="K210" s="1"/>
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B211" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D211" t="str">
         <f>""</f>
@@ -9328,10 +9321,10 @@
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B212" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D212" t="str">
         <f>""</f>
@@ -9356,18 +9349,18 @@
       <c r="J212" s="1"/>
       <c r="K212" s="1"/>
       <c r="N212" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B213" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C213" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D213" t="str">
         <f>"0062409166"</f>
@@ -9394,10 +9387,10 @@
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B214" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D214" t="str">
         <f>"1101886722"</f>
@@ -9424,10 +9417,10 @@
     </row>
     <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B215" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D215" t="str">
         <f>""</f>
@@ -9451,10 +9444,10 @@
     </row>
     <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B216" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D216" t="str">
         <f>""</f>
@@ -9481,10 +9474,10 @@
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B217" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D217" t="str">
         <f>""</f>
@@ -9511,10 +9504,10 @@
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B218" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D218" t="str">
         <f>"0008172145"</f>
@@ -9540,10 +9533,10 @@
     </row>
     <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B219" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D219" t="str">
         <f>"0062659057"</f>
@@ -9569,10 +9562,10 @@
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B220" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D220" t="str">
         <f>"1947870009"</f>
@@ -9595,16 +9588,16 @@
         <v>2023</v>
       </c>
       <c r="J220" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="K220" s="1"/>
     </row>
     <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B221" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D221" t="str">
         <f>""</f>
@@ -9629,18 +9622,18 @@
       <c r="J221" s="1"/>
       <c r="K221" s="1"/>
       <c r="N221" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B222" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C222" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D222" t="str">
         <f>"1538760533"</f>
@@ -9663,18 +9656,18 @@
         <v>2020</v>
       </c>
       <c r="J222" s="1" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="K222" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B223" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D223" t="str">
         <f>"1501103474"</f>
@@ -9701,10 +9694,10 @@
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B224" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D224" t="str">
         <f>""</f>
@@ -9727,18 +9720,18 @@
         <v>2021</v>
       </c>
       <c r="J224" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="K224" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B225" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D225" t="str">
         <f>"0316475408"</f>
@@ -9761,16 +9754,16 @@
         <v>2021</v>
       </c>
       <c r="J225" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="K225" s="1"/>
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B226" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D226" t="str">
         <f>"0544416708"</f>
@@ -9793,16 +9786,16 @@
         <v>2023</v>
       </c>
       <c r="J226" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="K226" s="1"/>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B227" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D227" t="str">
         <f>"1538730391"</f>
@@ -9829,10 +9822,10 @@
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B228" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D228" t="str">
         <f>"1846144930"</f>
@@ -9859,10 +9852,10 @@
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B229" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D229" t="str">
         <f>"0571321941"</f>
@@ -9889,13 +9882,13 @@
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B230" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C230" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D230" t="str">
         <f>""</f>
@@ -9920,15 +9913,15 @@
       <c r="J230" s="1"/>
       <c r="K230" s="1"/>
       <c r="N230" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B231" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D231" t="str">
         <f>"0241293863"</f>
@@ -9955,10 +9948,10 @@
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B232" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D232" t="str">
         <f>"1250304865"</f>
@@ -9983,18 +9976,18 @@
       <c r="J232" s="1"/>
       <c r="K232" s="1"/>
       <c r="N232" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B233" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C233" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D233" t="str">
         <f>"1542042062"</f>
@@ -10017,19 +10010,19 @@
         <v>2021</v>
       </c>
       <c r="J233" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="K233" s="1"/>
       <c r="N233" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B234" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D234" t="str">
         <f>"1783784849"</f>
@@ -10056,10 +10049,10 @@
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B235" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D235" t="str">
         <f>"1937512770"</f>
@@ -10086,10 +10079,10 @@
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B236" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D236" t="str">
         <f>""</f>
@@ -10116,10 +10109,10 @@
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B237" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D237" t="str">
         <f>"0525558756"</f>
@@ -10146,10 +10139,10 @@
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B238" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D238" t="str">
         <f>""</f>
@@ -10176,10 +10169,10 @@
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B239" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D239" t="str">
         <f>""</f>
@@ -10206,10 +10199,10 @@
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B240" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D240" t="str">
         <f>"0812994167"</f>
@@ -10236,13 +10229,13 @@
     </row>
     <row r="241" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B241" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C241" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D241" t="str">
         <f>""</f>
@@ -10268,10 +10261,10 @@
     </row>
     <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B242" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D242" t="str">
         <f>""</f>
@@ -10298,10 +10291,10 @@
     </row>
     <row r="243" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B243" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D243" t="str">
         <f>""</f>
@@ -10328,13 +10321,13 @@
     </row>
     <row r="244" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B244" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C244" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D244" t="str">
         <f>"0593169344"</f>
@@ -10361,10 +10354,10 @@
     </row>
     <row r="245" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B245" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D245" t="str">
         <f>"0525539557"</f>
@@ -10387,21 +10380,21 @@
         <v>2021</v>
       </c>
       <c r="J245" s="1" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="K245" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="N245" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B246" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D246" t="str">
         <f>"1487006500"</f>
@@ -10428,10 +10421,10 @@
     </row>
     <row r="247" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B247" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D247" t="str">
         <f>""</f>
@@ -10458,10 +10451,10 @@
     </row>
     <row r="248" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B248" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D248" t="str">
         <f>"0310109604"</f>
@@ -10482,15 +10475,15 @@
       </c>
       <c r="J248" s="1"/>
       <c r="K248" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="249" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B249" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D249" t="str">
         <f>"0691178704"</f>
@@ -10513,18 +10506,18 @@
         <v>2021</v>
       </c>
       <c r="J249" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="K249" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="250" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B250" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D250" t="str">
         <f>"1250266491"</f>
@@ -10551,10 +10544,10 @@
     </row>
     <row r="251" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B251" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D251" t="str">
         <f>"039354091X"</f>
@@ -10581,10 +10574,10 @@
     </row>
     <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B252" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D252" t="str">
         <f>""</f>
@@ -10604,22 +10597,22 @@
         <v>2023</v>
       </c>
       <c r="J252" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="K252" s="1"/>
       <c r="N252" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="253" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B253" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C253" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D253" t="str">
         <f>"067491919X"</f>
@@ -10642,21 +10635,21 @@
         <v>2021</v>
       </c>
       <c r="J253" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="K253" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="N253" t="s">
         <v>571</v>
-      </c>
-      <c r="K253" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="N253" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="254" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B254" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D254" t="str">
         <f>"1643138391"</f>
@@ -10683,10 +10676,10 @@
     </row>
     <row r="255" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="B255" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D255" t="str">
         <f>""</f>
@@ -10707,10 +10700,10 @@
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B256" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D256" t="str">
         <f>""</f>
@@ -10737,10 +10730,10 @@
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B257" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D257" t="str">
         <f>""</f>
@@ -10767,10 +10760,10 @@
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B258" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D258" t="str">
         <f>"1118411579"</f>
@@ -10793,24 +10786,24 @@
         <v>2018</v>
       </c>
       <c r="J258" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="K258" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M258" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B259" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C259" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D259" t="str">
         <f>"1472960181"</f>
@@ -10833,18 +10826,18 @@
         <v>2020</v>
       </c>
       <c r="J259" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K259" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B260" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D260" t="str">
         <f>"1925591697"</f>
@@ -10867,18 +10860,18 @@
         <v>2020</v>
       </c>
       <c r="J260" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K260" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B261" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D261" t="str">
         <f>"1786271974"</f>
@@ -10901,18 +10894,18 @@
         <v>2021</v>
       </c>
       <c r="J261" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="K261" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B262" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D262" t="str">
         <f>"1869661346"</f>
@@ -10935,18 +10928,18 @@
         <v>2021</v>
       </c>
       <c r="J262" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K262" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="263" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B263" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D263" t="str">
         <f>"192532205X"</f>
@@ -10969,19 +10962,19 @@
         <v>2021</v>
       </c>
       <c r="J263" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="K263" s="1"/>
     </row>
     <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B264" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C264" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D264" t="str">
         <f>"8417268073"</f>
@@ -11004,16 +10997,16 @@
         <v>2021</v>
       </c>
       <c r="J264" s="1" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="K264" s="1"/>
     </row>
     <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B265" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D265" t="str">
         <f>""</f>
@@ -11036,21 +11029,21 @@
         <v>2021</v>
       </c>
       <c r="J265" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K265" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="B266" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="C266" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="E266">
         <v>9788120801646</v>
@@ -11068,21 +11061,21 @@
         <v>2023</v>
       </c>
       <c r="J266" s="1" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
       <c r="K266" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M266" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="B267" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="E267">
         <v>9788123767598</v>
@@ -11100,21 +11093,21 @@
         <v>2023</v>
       </c>
       <c r="J267" s="1" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="K267" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M267" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="B268" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="E268">
         <v>9788171566662</v>
@@ -11132,21 +11125,21 @@
         <v>2023</v>
       </c>
       <c r="J268" s="1" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="K268" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M268" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
       <c r="B269" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="E269">
         <v>9789389924947</v>
@@ -11164,21 +11157,21 @@
         <v>2023</v>
       </c>
       <c r="J269" s="1" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="K269" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M269" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
       <c r="B270" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
       <c r="D270" s="4">
         <v>9358892021</v>
@@ -11199,21 +11192,21 @@
         <v>2023</v>
       </c>
       <c r="J270" s="1" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="K270" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M270" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="B271" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="E271">
         <v>9789394168961</v>
@@ -11228,13 +11221,172 @@
         <v>2023</v>
       </c>
       <c r="J271" s="1" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="K271" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="M271" t="s">
-        <v>563</v>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>575</v>
+      </c>
+      <c r="B272" t="s">
+        <v>371</v>
+      </c>
+      <c r="I272">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>579</v>
+      </c>
+      <c r="B273" t="s">
+        <v>371</v>
+      </c>
+      <c r="I273">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>580</v>
+      </c>
+      <c r="B274" t="s">
+        <v>371</v>
+      </c>
+      <c r="I274">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>581</v>
+      </c>
+      <c r="B275" t="s">
+        <v>371</v>
+      </c>
+      <c r="I275">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>582</v>
+      </c>
+      <c r="B276" t="s">
+        <v>371</v>
+      </c>
+      <c r="I276">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>583</v>
+      </c>
+      <c r="B277" t="s">
+        <v>371</v>
+      </c>
+      <c r="I277">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>584</v>
+      </c>
+      <c r="B278" t="s">
+        <v>371</v>
+      </c>
+      <c r="I278">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>585</v>
+      </c>
+      <c r="B279" t="s">
+        <v>255</v>
+      </c>
+      <c r="I279">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>586</v>
+      </c>
+      <c r="B280" t="s">
+        <v>255</v>
+      </c>
+      <c r="I280">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>587</v>
+      </c>
+      <c r="B281" t="s">
+        <v>255</v>
+      </c>
+      <c r="I281">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>588</v>
+      </c>
+      <c r="B282" t="s">
+        <v>255</v>
+      </c>
+      <c r="I282">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>572</v>
+      </c>
+      <c r="B283" t="s">
+        <v>573</v>
+      </c>
+      <c r="I283">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>546</v>
+      </c>
+      <c r="B284" t="s">
+        <v>547</v>
+      </c>
+      <c r="I284">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>548</v>
+      </c>
+      <c r="B285" t="s">
+        <v>549</v>
+      </c>
+      <c r="I285">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>608</v>
       </c>
     </row>
   </sheetData>
@@ -11245,202 +11397,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC92D16A-4E74-AC46-8BF1-3DC9B87B009C}">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView zoomScale="226" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>589</v>
-      </c>
-      <c r="C1" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>549</v>
-      </c>
-      <c r="C2">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>550</v>
-      </c>
-      <c r="B3" t="s">
-        <v>551</v>
-      </c>
-      <c r="C3">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>552</v>
-      </c>
-      <c r="B4" t="s">
-        <v>553</v>
-      </c>
-      <c r="C4">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>581</v>
-      </c>
-      <c r="B5" t="s">
-        <v>582</v>
-      </c>
-      <c r="C5">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>585</v>
-      </c>
-      <c r="B7" t="s">
-        <v>374</v>
-      </c>
-      <c r="C7">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>590</v>
-      </c>
-      <c r="B8" t="s">
-        <v>374</v>
-      </c>
-      <c r="C8">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>591</v>
-      </c>
-      <c r="B9" t="s">
-        <v>374</v>
-      </c>
-      <c r="C9">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>592</v>
-      </c>
-      <c r="B10" t="s">
-        <v>374</v>
-      </c>
-      <c r="C10">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>593</v>
-      </c>
-      <c r="B11" t="s">
-        <v>374</v>
-      </c>
-      <c r="C11">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>594</v>
-      </c>
-      <c r="B12" t="s">
-        <v>374</v>
-      </c>
-      <c r="C12">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>595</v>
-      </c>
-      <c r="B13" t="s">
-        <v>374</v>
-      </c>
-      <c r="C13">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>596</v>
-      </c>
-      <c r="B14" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>597</v>
-      </c>
-      <c r="B15" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>598</v>
-      </c>
-      <c r="B16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C16">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>599</v>
-      </c>
-      <c r="B17" t="s">
-        <v>258</v>
-      </c>
-      <c r="C17">
-        <v>2014</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>